<commit_message>
Adicionando planning poker no planejamento geral
</commit_message>
<xml_diff>
--- a/docs/planejamentoGeral.xlsx
+++ b/docs/planejamentoGeral.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unifmgomes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Unifdmiranda\Downloads\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F1425F-D88D-4325-AC6C-2E1DE8CABE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87CA0A27-5EAB-4171-82FD-ADBCB6B90306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{8F403C45-E478-4B19-AACD-B09D2859DD5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8F403C45-E478-4B19-AACD-B09D2859DD5D}"/>
   </bookViews>
   <sheets>
     <sheet name="INVEST" sheetId="1" r:id="rId1"/>
     <sheet name="MOSCOW" sheetId="3" r:id="rId2"/>
-    <sheet name="PRIORIZAÇÃO" sheetId="2" r:id="rId3"/>
+    <sheet name="PRIORIZAÇÃO E PONTUAÇÃO" sheetId="2" r:id="rId3"/>
     <sheet name="CRITÉRIOS DE ACEITE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="168">
   <si>
     <t>gestão financeira</t>
   </si>
@@ -511,13 +511,46 @@
   </si>
   <si>
     <t>o sistema não deve atualizar as estatísticas</t>
+  </si>
+  <si>
+    <t>SPRINT 1</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Pontos da História</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>Cadastro/Login na plataforma</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>Cadastrar/editar movimentações financeiras</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>Visualizar estatísticas financeiras e consulta sobre situação</t>
+  </si>
+  <si>
+    <t>Pontos de História</t>
+  </si>
+  <si>
+    <t>BACKLOG GERAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,8 +564,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -569,6 +610,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -750,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -762,24 +809,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -836,6 +865,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -845,11 +892,232 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="33">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -862,11 +1130,13 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -966,13 +1236,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -998,6 +1261,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1005,16 +1275,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1023,6 +1284,12 @@
         </right>
         <top/>
         <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1168,25 +1435,53 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1203,25 +1498,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D418BAD3-138F-4BCC-9F6E-FECC93CAF7C8}" name="Tabela3" displayName="Tabela3" ref="B2:G14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D418BAD3-138F-4BCC-9F6E-FECC93CAF7C8}" name="Tabela3" displayName="Tabela3" ref="B2:G14" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0C7B1354-065A-4F0D-99E9-D63EA7B7A3FB}" name="ID" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{603F40D7-E879-4AB9-B9B7-122E785DBF18}" name="História" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{206574EF-25C4-41B8-AA55-DC9304334183}" name="M" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{88E4E1E8-2FB2-41F4-95A7-1947017B59AC}" name="S" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{8E7FB667-1BE4-4F40-98AA-436AC3D3D4D9}" name="C" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{6588A67C-1B4D-4B58-9EAA-53910530A15F}" name="W" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{0C7B1354-065A-4F0D-99E9-D63EA7B7A3FB}" name="ID" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{603F40D7-E879-4AB9-B9B7-122E785DBF18}" name="História" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{206574EF-25C4-41B8-AA55-DC9304334183}" name="M" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{88E4E1E8-2FB2-41F4-95A7-1947017B59AC}" name="S" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{8E7FB667-1BE4-4F40-98AA-436AC3D3D4D9}" name="C" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{6588A67C-1B4D-4B58-9EAA-53910530A15F}" name="W" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{647DB52C-394A-4B15-B209-60DE7A1DC124}" name="Tabela35" displayName="Tabela35" ref="B2:D14" totalsRowShown="0" headerRowDxfId="0" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{98F2D7FF-AD24-4473-8342-8D6EF05365F6}" name="ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{D0168E4D-23F4-4A35-9DA5-69876964CCA6}" name="História" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{D146CA91-2579-4EB4-80F8-EA924749846B}" name="Prioridade" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{647DB52C-394A-4B15-B209-60DE7A1DC124}" name="Tabela35" displayName="Tabela35" ref="B5:E17" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{98F2D7FF-AD24-4473-8342-8D6EF05365F6}" name="ID" totalsRowLabel="Total" dataDxfId="16" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{D0168E4D-23F4-4A35-9DA5-69876964CCA6}" name="História" dataDxfId="15" totalsRowDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{D146CA91-2579-4EB4-80F8-EA924749846B}" name="Prioridade" dataDxfId="14" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{F81E1A7E-DE27-4D2D-910A-D6E9CF9AD569}" name="Pontos de História" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67CC093D-9138-458A-BB2A-2E501DE77F21}" name="Tabela43" displayName="Tabela43" ref="B20:E23" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="7">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F3A3E39C-2785-4879-B14E-F7EAF31E5DA0}" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{1C46741D-9668-4710-BF62-9A6A244250E0}" name="Descrição" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{8AEF3AF3-E1A3-4960-A5A4-A6F0C0C90EEE}" name="Prioridade" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{54A57216-D5FF-4826-82B3-BE00513B887E}" name="Pontos da História" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1538,41 +1846,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1598,10 +1906,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1624,10 +1932,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1657,38 +1965,38 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1717,7 +2025,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1743,7 +2051,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1767,7 +2075,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1791,7 +2099,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1815,7 +2123,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1839,7 +2147,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1874,38 +2182,38 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1934,7 +2242,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1960,7 +2268,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1984,7 +2292,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2008,7 +2316,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2055,213 +2363,213 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="17"/>
-    <col min="2" max="2" width="5.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="135.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="18.28515625" style="17"/>
+    <col min="1" max="1" width="18.28515625" style="11"/>
+    <col min="2" max="2" width="5.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="135.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="18.28515625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="16"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23" t="s">
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="H10" s="16"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23" t="s">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="16"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23" t="s">
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="H12" s="16"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="16"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26" t="s">
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2276,168 +2584,267 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26068D64-6F76-40D3-8144-2942D514E32D}">
-  <dimension ref="B2:D14"/>
+  <dimension ref="B4:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="11"/>
-    <col min="2" max="2" width="5.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="136.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="136.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D5" s="14" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="E5" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C6" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D6" s="17" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="E6" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C7" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D7" s="17" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C8" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D8" s="17" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="E8" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C9" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D9" s="17" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C10" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D10" s="17" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C11" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D11" s="17" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="E11" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C12" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D12" s="17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C13" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D13" s="17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C14" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D14" s="17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C15" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D15" s="17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C16" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D16" s="17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C17" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D17" s="20" t="s">
         <v>108</v>
       </c>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="20">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B4:E4"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2446,29 +2853,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38A9823-1336-4F70-ADEA-3082FCEA272B}">
   <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.140625" defaultRowHeight="54" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="32.140625" style="11"/>
+    <col min="1" max="16384" width="32.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="21" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2476,16 +2883,16 @@
       <c r="B3" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="22" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2523,16 +2930,16 @@
       <c r="B6" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="22" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2555,16 +2962,16 @@
       <c r="B8" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="22" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2587,16 +2994,16 @@
       <c r="B10" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="22" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2619,16 +3026,16 @@
       <c r="B12" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="22" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2651,16 +3058,16 @@
       <c r="B14" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="22" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2681,12 +3088,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>